<commit_message>
Update Thiết kế giao diện - Trần Trung Tấn.xlsx
</commit_message>
<xml_diff>
--- a/Thiết kế/Thiết kế giao diện/Trung Tấn/Thiết kế giao diện - Trần Trung Tấn.xlsx
+++ b/Thiết kế/Thiết kế giao diện/Trung Tấn/Thiết kế giao diện - Trần Trung Tấn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Dropbox\My PC (LAPTOP-3KL3D18R)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\CNPM\Thiết kế\Thiết kế giao diện\Trung Tấn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7A6472-E78E-4A6D-B12D-AF2A1EB115B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD35A3DE-DF75-4DF0-85B3-2DDC08021968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99CC5337-4F64-435E-8CE4-9D32476A458D}"/>
+    <workbookView xWindow="1560" yWindow="1350" windowWidth="24810" windowHeight="14250" activeTab="2" xr2:uid="{99CC5337-4F64-435E-8CE4-9D32476A458D}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh mục nhân viên" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="337">
   <si>
     <t>Danh sách các biến cố</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Chọn nhân viên</t>
-  </si>
-  <si>
-    <t>Hiện trang thông tin nhân viên</t>
   </si>
   <si>
     <t>Chọn trang</t>
@@ -362,9 +359,6 @@
     <t>Chọn đơn hàng</t>
   </si>
   <si>
-    <t>Hiện trang thông tin đơn hàng</t>
-  </si>
-  <si>
     <t>Đọc danh sách đơn hàng từ CSDL
 Xuất danh sách đơn hàng</t>
   </si>
@@ -1009,6 +1003,54 @@
   </si>
   <si>
     <t xml:space="preserve">Hiển thị tiêu đề Tổng tiền </t>
+  </si>
+  <si>
+    <t>Chọn nút Lịch làm</t>
+  </si>
+  <si>
+    <t>Chọn nút Tính lương</t>
+  </si>
+  <si>
+    <t>Bt_Lichlam</t>
+  </si>
+  <si>
+    <t>Bt_Tinhluong</t>
+  </si>
+  <si>
+    <t>Hiện cửa sổ Lịch làm</t>
+  </si>
+  <si>
+    <t>Hiện cửa sổ Tính lương</t>
+  </si>
+  <si>
+    <t>Hiển thị cửa sổ Lịch làm</t>
+  </si>
+  <si>
+    <t>Hiển thị cửa sổ Tính lương</t>
+  </si>
+  <si>
+    <t>Chọn nút xóa</t>
+  </si>
+  <si>
+    <t>Chọn lịch làm nhân viên</t>
+  </si>
+  <si>
+    <t>Hiện cửa sổ thông tin nhân viên</t>
+  </si>
+  <si>
+    <t>Hiện cửa sổ  thông tin đơn hàng</t>
+  </si>
+  <si>
+    <t>Hiện cửa sổ check in</t>
+  </si>
+  <si>
+    <t>Xóa lịch làm</t>
+  </si>
+  <si>
+    <t>Lb_Calam</t>
+  </si>
+  <si>
+    <t>Chọn xem check in nhân viên</t>
   </si>
 </sst>
 </file>
@@ -1320,35 +1362,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1367,12 +1385,43 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1388,13 +1437,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1416,23 +1458,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2978966</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5D96A22-C2E0-4EAB-A6E1-ABF8B105F3E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8655FA3-FE03-4A58-AC2A-84EEE3C7A0FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1455,8 +1497,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="619125" y="190500"/>
-          <a:ext cx="9094016" cy="4124325"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13239750" cy="5010150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1610,22 +1652,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>195263</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E44A0B2-9E06-45A4-94B9-657BBB604D2E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{062A246C-BA12-4D76-BDD0-149D5C2E9D04}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1648,8 +1690,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="152400" y="11287125"/>
-          <a:ext cx="12249150" cy="5838825"/>
+          <a:off x="0" y="12915900"/>
+          <a:ext cx="11572875" cy="5419725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2234,8 +2276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA08774-5637-4D8E-BC2A-0903C8831B06}">
   <dimension ref="A28:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2243,7 +2285,7 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="9.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="55.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
@@ -2252,13 +2294,13 @@
   </cols>
   <sheetData>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2349,7 +2391,7 @@
         <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>16</v>
+        <v>331</v>
       </c>
       <c r="E35" s="3"/>
     </row>
@@ -2359,10 +2401,10 @@
         <v>6</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="E36" s="3"/>
     </row>
@@ -2372,10 +2414,10 @@
         <v>7</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="E37" s="3"/>
     </row>
@@ -2385,116 +2427,89 @@
         <v>8</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3">
+        <v>9</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3">
+        <v>10</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E40" s="3"/>
+    </row>
+    <row r="42" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="7"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3">
-        <v>2</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="26"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="3">
-        <v>3</v>
+      <c r="B44" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>113</v>
+        <v>28</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>117</v>
+        <v>55</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -2503,16 +2518,16 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2521,16 +2536,16 @@
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2539,16 +2554,16 @@
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -2557,16 +2572,16 @@
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -2575,16 +2590,16 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -2593,16 +2608,16 @@
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -2611,16 +2626,16 @@
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -2629,16 +2644,16 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -2647,16 +2662,16 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -2665,16 +2680,16 @@
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -2683,29 +2698,119 @@
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3">
+        <v>13</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3">
+        <v>14</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3">
+        <v>15</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3">
+        <v>16</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3">
+        <v>17</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+    </row>
     <row r="92" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="18"/>
+      <c r="D97" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A40:H40"/>
+    <mergeCell ref="A43:H43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2718,7 +2823,7 @@
   <dimension ref="A26:G55"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2733,164 +2838,164 @@
   </cols>
   <sheetData>
     <row r="26" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="23">
+      <c r="A28" s="15">
         <v>0</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>2</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="1:4" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
-        <v>2</v>
-      </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>3</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23">
-        <v>3</v>
-      </c>
-      <c r="B31" s="3" t="s">
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="23">
-        <v>4</v>
-      </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>5</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="1:7" ht="33" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
-        <v>5</v>
-      </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>6</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>7</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="12">
-        <v>6</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="13"/>
+        <v>332</v>
+      </c>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14">
+      <c r="A36" s="7">
         <v>8</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D36" s="16"/>
+        <v>107</v>
+      </c>
+      <c r="D36" s="9"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
+      <c r="A39" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="E40" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>4</v>
@@ -2901,13 +3006,13 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -2918,13 +3023,13 @@
         <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -2935,13 +3040,13 @@
         <v>3</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -2952,13 +3057,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -2969,13 +3074,13 @@
         <v>5</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -2986,13 +3091,13 @@
         <v>6</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -3003,13 +3108,13 @@
         <v>7</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -3020,13 +3125,13 @@
         <v>8</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3037,13 +3142,13 @@
         <v>9</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -3054,13 +3159,13 @@
         <v>10</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -3071,13 +3176,13 @@
         <v>11</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -3088,13 +3193,13 @@
         <v>12</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -3105,13 +3210,13 @@
         <v>13</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -3122,13 +3227,13 @@
         <v>14</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -3139,13 +3244,13 @@
         <v>15</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -3163,10 +3268,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AB9B7F-5532-466A-8C88-B1D000186150}">
-  <dimension ref="A31:G101"/>
+  <dimension ref="A31:G105"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3174,7 +3279,7 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="41.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="54.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" style="2" customWidth="1"/>
@@ -3184,13 +3289,13 @@
   </cols>
   <sheetData>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="11"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -3212,10 +3317,10 @@
         <v>0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -3225,10 +3330,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -3238,10 +3343,10 @@
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -3254,7 +3359,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -3264,10 +3369,10 @@
         <v>4</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -3277,41 +3382,41 @@
         <v>5</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
+      <c r="A42" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>4</v>
@@ -3322,13 +3427,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -3339,13 +3444,13 @@
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -3356,13 +3461,13 @@
         <v>3</v>
       </c>
       <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -3373,13 +3478,13 @@
         <v>4</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -3390,13 +3495,13 @@
         <v>5</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3407,13 +3512,13 @@
         <v>6</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -3424,13 +3529,13 @@
         <v>7</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -3441,13 +3546,13 @@
         <v>8</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -3458,13 +3563,13 @@
         <v>9</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -3475,25 +3580,25 @@
         <v>10</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
+      <c r="A87" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B87" s="28"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
@@ -3517,7 +3622,7 @@
         <v>13</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D89" s="3"/>
     </row>
@@ -3526,10 +3631,10 @@
         <v>1</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D90" s="3"/>
     </row>
@@ -3538,10 +3643,10 @@
         <v>2</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D91" s="3"/>
     </row>
@@ -3550,93 +3655,83 @@
         <v>3</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="D92" s="3"/>
     </row>
+    <row r="93" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>4</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" s="3"/>
+    </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A94" s="3">
+        <v>5</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D94" s="3"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B96" s="28"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
+      <c r="G96" s="28"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="B97" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="D97" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="E97" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="F97" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G95" s="3" t="s">
+      <c r="G97" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
-        <v>1</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="3">
-        <v>2</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
@@ -3644,16 +3739,16 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
@@ -3661,16 +3756,16 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="D100" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
@@ -3678,27 +3773,95 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>5</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="3">
+        <v>6</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="3">
+        <v>7</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="3">
+        <v>8</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A31:E31"/>
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="A96:G96"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3727,354 +3890,354 @@
   </cols>
   <sheetData>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="A22" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+      <c r="A23" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="18"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="28" t="s">
+      <c r="B26" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="27"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="28" t="s">
+      <c r="D26" s="18"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B26" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="27" t="s">
+      <c r="B27" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D26" s="27"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="28" t="s">
+      <c r="D27" s="18"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="D27" s="27"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="27"/>
+      <c r="D28" s="18"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="36"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="27" t="s">
+      <c r="C32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="D32" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="E32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="26">
+      <c r="A33" s="17">
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>2</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>3</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <v>5</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="26">
-        <v>2</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="26">
-        <v>3</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="26">
-        <v>4</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
-        <v>5</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C38" s="27" t="s">
+      <c r="A38" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
-        <v>138</v>
+      <c r="A39" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="18" t="s">
         <v>139</v>
-      </c>
-      <c r="B40" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>141</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="B41" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>143</v>
+      <c r="A41" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>141</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>153</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>149</v>
+      <c r="A42" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
-        <v>144</v>
+      <c r="A43" s="17" t="s">
+        <v>142</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>37</v>
+        <v>155</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>37</v>
+      <c r="A44" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>37</v>
+      <c r="A45" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B46" s="27" t="s">
+      <c r="A46" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -4095,7 +4258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75723C6B-E813-4725-B3A6-1E09678B960F}">
   <dimension ref="A32:G74"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
@@ -4112,12 +4275,12 @@
   </cols>
   <sheetData>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -4138,10 +4301,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>160</v>
+        <v>157</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>158</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -4150,10 +4313,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>173</v>
+        <v>159</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>171</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -4162,10 +4325,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>174</v>
+        <v>163</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>172</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -4174,10 +4337,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -4186,10 +4349,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D38" s="3"/>
     </row>
@@ -4198,10 +4361,10 @@
         <v>5</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -4210,10 +4373,10 @@
         <v>6</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>175</v>
+        <v>164</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -4222,10 +4385,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>176</v>
+        <v>165</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -4234,10 +4397,10 @@
         <v>8</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>177</v>
+        <v>166</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -4246,10 +4409,10 @@
         <v>9</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>178</v>
+        <v>167</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D43" s="3"/>
     </row>
@@ -4258,10 +4421,10 @@
         <v>10</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>179</v>
+        <v>168</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="D44" s="3"/>
     </row>
@@ -4282,10 +4445,10 @@
         <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>183</v>
+        <v>160</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="D46" s="3"/>
     </row>
@@ -4294,42 +4457,42 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>184</v>
+        <v>161</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="32" t="s">
+      <c r="A49" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="27" t="s">
+      <c r="C50" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C50" s="27" t="s">
+      <c r="D50" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="27" t="s">
+      <c r="E50" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>4</v>
@@ -4339,14 +4502,14 @@
       <c r="A51" s="3">
         <v>1</v>
       </c>
-      <c r="B51" s="27" t="s">
-        <v>137</v>
-      </c>
-      <c r="C51" s="27" t="s">
+      <c r="B51" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -4356,33 +4519,33 @@
       <c r="A52" s="3">
         <v>2</v>
       </c>
-      <c r="B52" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="C52" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>195</v>
+      <c r="B52" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>193</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="34" t="s">
-        <v>279</v>
+      <c r="G52" s="20" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>3</v>
       </c>
-      <c r="B53" s="27" t="s">
-        <v>186</v>
-      </c>
-      <c r="C53" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>196</v>
+      <c r="B53" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>194</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -4392,14 +4555,14 @@
       <c r="A54" s="3">
         <v>4</v>
       </c>
-      <c r="B54" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="C54" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>197</v>
+      <c r="B54" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -4409,14 +4572,14 @@
       <c r="A55" s="3">
         <v>5</v>
       </c>
-      <c r="B55" s="27" t="s">
-        <v>188</v>
-      </c>
-      <c r="C55" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>198</v>
+      <c r="B55" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>196</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -4426,14 +4589,14 @@
       <c r="A56" s="3">
         <v>6</v>
       </c>
-      <c r="B56" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C56" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>199</v>
+      <c r="B56" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>197</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -4443,14 +4606,14 @@
       <c r="A57" s="3">
         <v>7</v>
       </c>
-      <c r="B57" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>200</v>
+      <c r="B57" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>198</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -4460,14 +4623,14 @@
       <c r="A58" s="3">
         <v>8</v>
       </c>
-      <c r="B58" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>201</v>
+      <c r="B58" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>199</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -4477,14 +4640,14 @@
       <c r="A59" s="3">
         <v>9</v>
       </c>
-      <c r="B59" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>202</v>
+      <c r="B59" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>200</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -4494,14 +4657,14 @@
       <c r="A60" s="3">
         <v>10</v>
       </c>
-      <c r="B60" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="C60" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>203</v>
+      <c r="B60" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -4511,14 +4674,14 @@
       <c r="A61" s="3">
         <v>11</v>
       </c>
-      <c r="B61" s="27" t="s">
-        <v>194</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>204</v>
+      <c r="B61" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>202</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -4529,13 +4692,13 @@
         <v>12</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -4546,13 +4709,13 @@
         <v>13</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -4563,13 +4726,13 @@
         <v>14</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -4580,13 +4743,13 @@
         <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -4597,13 +4760,13 @@
         <v>16</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -4614,13 +4777,13 @@
         <v>17</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -4630,14 +4793,14 @@
       <c r="A68" s="3">
         <v>18</v>
       </c>
-      <c r="B68" s="27" t="s">
-        <v>231</v>
+      <c r="B68" s="18" t="s">
+        <v>229</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D68" s="27" t="s">
-        <v>239</v>
+        <v>230</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>237</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -4647,14 +4810,14 @@
       <c r="A69" s="3">
         <v>19</v>
       </c>
-      <c r="B69" s="27" t="s">
-        <v>233</v>
+      <c r="B69" s="18" t="s">
+        <v>231</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D69" s="27" t="s">
-        <v>240</v>
+        <v>230</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -4664,14 +4827,14 @@
       <c r="A70" s="3">
         <v>20</v>
       </c>
-      <c r="B70" s="27" t="s">
-        <v>234</v>
+      <c r="B70" s="18" t="s">
+        <v>232</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D70" s="27" t="s">
-        <v>241</v>
+        <v>230</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>239</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -4681,14 +4844,14 @@
       <c r="A71" s="3">
         <v>21</v>
       </c>
-      <c r="B71" s="27" t="s">
-        <v>235</v>
+      <c r="B71" s="18" t="s">
+        <v>233</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D71" s="27" t="s">
-        <v>242</v>
+        <v>230</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -4698,14 +4861,14 @@
       <c r="A72" s="3">
         <v>22</v>
       </c>
-      <c r="B72" s="27" t="s">
-        <v>236</v>
+      <c r="B72" s="18" t="s">
+        <v>234</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>243</v>
+        <v>230</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>241</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -4715,14 +4878,14 @@
       <c r="A73" s="3">
         <v>23</v>
       </c>
-      <c r="B73" s="27" t="s">
-        <v>237</v>
+      <c r="B73" s="18" t="s">
+        <v>235</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D73" s="27" t="s">
-        <v>244</v>
+        <v>230</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>242</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -4732,14 +4895,14 @@
       <c r="A74" s="3">
         <v>24</v>
       </c>
-      <c r="B74" s="27" t="s">
-        <v>238</v>
+      <c r="B74" s="18" t="s">
+        <v>236</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D74" s="27" t="s">
-        <v>245</v>
+        <v>230</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>243</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -4760,7 +4923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036D6770-D2E0-4CDD-A8DC-713867DC3285}">
   <dimension ref="A33:G67"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
@@ -4777,12 +4940,12 @@
   </cols>
   <sheetData>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -4803,10 +4966,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -4815,10 +4978,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -4827,10 +4990,10 @@
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -4839,10 +5002,10 @@
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D38" s="3"/>
     </row>
@@ -4851,10 +5014,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -4863,10 +5026,10 @@
         <v>5</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -4878,7 +5041,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -4887,10 +5050,10 @@
         <v>7</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -4899,42 +5062,42 @@
         <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>184</v>
+        <v>228</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B45" s="32"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="27" t="s">
+      <c r="C46" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="D46" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="27" t="s">
+      <c r="E46" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>4</v>
@@ -4944,14 +5107,14 @@
       <c r="A47" s="3">
         <v>1</v>
       </c>
-      <c r="B47" s="27" t="s">
-        <v>137</v>
+      <c r="B47" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -4961,33 +5124,33 @@
       <c r="A48" s="3">
         <v>2</v>
       </c>
-      <c r="B48" s="27" t="s">
-        <v>246</v>
+      <c r="B48" s="18" t="s">
+        <v>244</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>251</v>
+        <v>36</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>249</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="35" t="s">
-        <v>280</v>
+      <c r="G48" s="21" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>3</v>
       </c>
-      <c r="B49" s="27" t="s">
-        <v>247</v>
+      <c r="B49" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>252</v>
+        <v>36</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>250</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -4997,14 +5160,14 @@
       <c r="A50" s="3">
         <v>4</v>
       </c>
-      <c r="B50" s="27" t="s">
-        <v>248</v>
+      <c r="B50" s="18" t="s">
+        <v>246</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>299</v>
+        <v>36</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>297</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -5014,33 +5177,33 @@
       <c r="A51" s="3">
         <v>5</v>
       </c>
-      <c r="B51" s="27" t="s">
-        <v>249</v>
+      <c r="B51" s="18" t="s">
+        <v>247</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>253</v>
+        <v>36</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>251</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>6</v>
       </c>
-      <c r="B52" s="27" t="s">
-        <v>250</v>
+      <c r="B52" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>254</v>
+        <v>36</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>252</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -5050,14 +5213,14 @@
       <c r="A53" s="3">
         <v>7</v>
       </c>
-      <c r="B53" s="27" t="s">
-        <v>258</v>
+      <c r="B53" s="18" t="s">
+        <v>256</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>257</v>
+        <v>36</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -5068,13 +5231,13 @@
         <v>8</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -5084,14 +5247,14 @@
       <c r="A55" s="3">
         <v>9</v>
       </c>
-      <c r="B55" s="27" t="s">
-        <v>259</v>
+      <c r="B55" s="18" t="s">
+        <v>257</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>240</v>
+        <v>230</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>238</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -5101,14 +5264,14 @@
       <c r="A56" s="3">
         <v>10</v>
       </c>
-      <c r="B56" s="27" t="s">
-        <v>260</v>
+      <c r="B56" s="18" t="s">
+        <v>258</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>241</v>
+        <v>230</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>239</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -5118,14 +5281,14 @@
       <c r="A57" s="3">
         <v>11</v>
       </c>
-      <c r="B57" s="27" t="s">
-        <v>261</v>
+      <c r="B57" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>242</v>
+        <v>230</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>240</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -5135,14 +5298,14 @@
       <c r="A58" s="3">
         <v>12</v>
       </c>
-      <c r="B58" s="27" t="s">
-        <v>262</v>
+      <c r="B58" s="18" t="s">
+        <v>260</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>244</v>
+        <v>230</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>242</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -5153,13 +5316,13 @@
         <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C59" s="27" t="s">
-        <v>145</v>
+        <v>261</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -5170,13 +5333,13 @@
         <v>14</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -5187,13 +5350,13 @@
         <v>15</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5204,13 +5367,13 @@
         <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -5221,13 +5384,13 @@
         <v>17</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -5238,13 +5401,13 @@
         <v>18</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -5255,13 +5418,13 @@
         <v>19</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -5272,13 +5435,13 @@
         <v>20</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -5289,13 +5452,13 @@
         <v>21</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -5330,12 +5493,12 @@
   </cols>
   <sheetData>
     <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -5356,10 +5519,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -5368,10 +5531,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -5380,22 +5543,22 @@
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="36">
+      <c r="A38" s="22">
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -5403,10 +5566,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -5415,10 +5578,10 @@
         <v>5</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -5430,7 +5593,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -5442,7 +5605,7 @@
         <v>15</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -5451,10 +5614,10 @@
         <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>290</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>292</v>
       </c>
       <c r="D43" s="3"/>
     </row>
@@ -5463,42 +5626,42 @@
         <v>9</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>184</v>
+        <v>228</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>182</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="A47" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+    </row>
+    <row r="48" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-    </row>
-    <row r="48" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="27" t="s">
+      <c r="C48" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="D48" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="27" t="s">
+      <c r="E48" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="G48" s="3" t="s">
         <v>4</v>
@@ -5508,14 +5671,14 @@
       <c r="A49" s="3">
         <v>1</v>
       </c>
-      <c r="B49" s="27" t="s">
-        <v>137</v>
+      <c r="B49" s="18" t="s">
+        <v>135</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="18" t="s">
         <v>37</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -5525,33 +5688,33 @@
       <c r="A50" s="3">
         <v>2</v>
       </c>
-      <c r="B50" s="27" t="s">
-        <v>293</v>
+      <c r="B50" s="18" t="s">
+        <v>291</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D50" s="27" t="s">
-        <v>294</v>
+        <v>36</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>292</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="35" t="s">
-        <v>295</v>
+      <c r="G50" s="21" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>3</v>
       </c>
-      <c r="B51" s="27" t="s">
-        <v>296</v>
+      <c r="B51" s="18" t="s">
+        <v>294</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>297</v>
+        <v>36</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>295</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -5561,14 +5724,14 @@
       <c r="A52" s="3">
         <v>4</v>
       </c>
-      <c r="B52" s="27" t="s">
-        <v>192</v>
+      <c r="B52" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>298</v>
+        <v>36</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>296</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -5578,33 +5741,33 @@
       <c r="A53" s="3">
         <v>5</v>
       </c>
-      <c r="B53" s="27" t="s">
-        <v>249</v>
+      <c r="B53" s="18" t="s">
+        <v>247</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>253</v>
+        <v>36</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>251</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>6</v>
       </c>
-      <c r="B54" s="27" t="s">
-        <v>193</v>
+      <c r="B54" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>203</v>
+        <v>36</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>201</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -5614,14 +5777,14 @@
       <c r="A55" s="3">
         <v>7</v>
       </c>
-      <c r="B55" s="27" t="s">
-        <v>258</v>
+      <c r="B55" s="18" t="s">
+        <v>256</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>257</v>
+        <v>36</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -5632,13 +5795,13 @@
         <v>8</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -5648,14 +5811,14 @@
       <c r="A57" s="3">
         <v>9</v>
       </c>
-      <c r="B57" s="27" t="s">
-        <v>301</v>
+      <c r="B57" s="18" t="s">
+        <v>299</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>302</v>
+        <v>230</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>300</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -5665,14 +5828,14 @@
       <c r="A58" s="3">
         <v>10</v>
       </c>
-      <c r="B58" s="27" t="s">
-        <v>303</v>
+      <c r="B58" s="18" t="s">
+        <v>301</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>304</v>
+        <v>230</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>302</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -5682,14 +5845,14 @@
       <c r="A59" s="3">
         <v>11</v>
       </c>
-      <c r="B59" s="27" t="s">
-        <v>236</v>
+      <c r="B59" s="18" t="s">
+        <v>234</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D59" s="27" t="s">
-        <v>305</v>
+        <v>230</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>303</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -5699,14 +5862,14 @@
       <c r="A60" s="3">
         <v>12</v>
       </c>
-      <c r="B60" s="27" t="s">
-        <v>237</v>
+      <c r="B60" s="18" t="s">
+        <v>235</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D60" s="27" t="s">
-        <v>244</v>
+        <v>230</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>242</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -5717,13 +5880,13 @@
         <v>13</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C61" s="27" t="s">
-        <v>145</v>
+        <v>261</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5734,13 +5897,13 @@
         <v>14</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -5751,13 +5914,13 @@
         <v>15</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -5768,13 +5931,13 @@
         <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -5785,13 +5948,13 @@
         <v>17</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -5802,13 +5965,13 @@
         <v>18</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -5819,81 +5982,81 @@
         <v>19</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="37">
+      <c r="A68" s="23">
         <v>20</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="37">
+      <c r="A69" s="23">
         <v>21</v>
       </c>
-      <c r="B69" s="37" t="s">
-        <v>317</v>
-      </c>
-      <c r="C69" s="37" t="s">
-        <v>37</v>
+      <c r="B69" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="37">
+      <c r="A70" s="23">
         <v>22</v>
       </c>
-      <c r="B70" s="37" t="s">
-        <v>319</v>
-      </c>
-      <c r="C70" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="D70" s="37" t="s">
-        <v>320</v>
+      <c r="B70" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="C70" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>318</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="37">
+      <c r="A71" s="23">
         <v>23</v>
       </c>
-      <c r="B71" s="37" t="s">
-        <v>321</v>
-      </c>
-      <c r="C71" s="37" t="s">
-        <v>37</v>
+      <c r="B71" s="23" t="s">
+        <v>319</v>
+      </c>
+      <c r="C71" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>

</xml_diff>

<commit_message>
Update và bổ sung
</commit_message>
<xml_diff>
--- a/Thiết kế/Thiết kế giao diện/Trung Tấn/Thiết kế giao diện - Trần Trung Tấn.xlsx
+++ b/Thiết kế/Thiết kế giao diện/Trung Tấn/Thiết kế giao diện - Trần Trung Tấn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\CNPM\Thiết kế\Thiết kế giao diện\Trung Tấn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD35A3DE-DF75-4DF0-85B3-2DDC08021968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF47D56A-A03C-4C2D-AA76-6DA97DF91C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1350" windowWidth="24810" windowHeight="14250" activeTab="2" xr2:uid="{99CC5337-4F64-435E-8CE4-9D32476A458D}"/>
+    <workbookView xWindow="2250" yWindow="1350" windowWidth="25230" windowHeight="14250" activeTab="1" xr2:uid="{99CC5337-4F64-435E-8CE4-9D32476A458D}"/>
   </bookViews>
   <sheets>
     <sheet name="Danh mục nhân viên" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="335">
   <si>
     <t>Danh sách các biến cố</t>
   </si>
@@ -347,13 +347,6 @@
   </si>
   <si>
     <t>Hiện form cập nhật đơn hàng</t>
-  </si>
-  <si>
-    <t>Chọn nút xóa đơn hàng</t>
-  </si>
-  <si>
-    <t>Hiện bảng xác nhận
-Nếu đồng ý thì xóa đơn hàng</t>
   </si>
   <si>
     <t>Chọn đơn hàng</t>
@@ -1097,7 +1090,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1291,21 +1284,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1354,7 +1332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1366,7 +1344,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1391,9 +1368,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1404,7 +1381,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1531,16 +1508,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>205185</xdr:colOff>
+      <xdr:colOff>22533</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB3949B9-8055-4023-A65E-B56D0F5B37E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FB35A7E-5746-44D1-AEC7-E01ABC6584CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1564,7 +1541,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="12639675" cy="4648200"/>
+          <a:ext cx="12452658" cy="4619625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2276,7 +2253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA08774-5637-4D8E-BC2A-0903C8831B06}">
   <dimension ref="A28:H97"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
@@ -2294,13 +2271,13 @@
   </cols>
   <sheetData>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="26"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
@@ -2391,7 +2368,7 @@
         <v>15</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E35" s="3"/>
     </row>
@@ -2440,10 +2417,10 @@
         <v>9</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E39" s="3"/>
     </row>
@@ -2453,25 +2430,25 @@
         <v>10</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E40" s="3"/>
     </row>
     <row r="42" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="24" t="s">
+      <c r="A43" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="26"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="25"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
@@ -2506,7 +2483,7 @@
         <v>28</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>55</v>
@@ -2521,13 +2498,13 @@
         <v>2</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -2539,13 +2516,13 @@
         <v>3</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -2557,13 +2534,13 @@
         <v>4</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -2719,13 +2696,13 @@
         <v>13</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -2737,13 +2714,13 @@
         <v>14</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -2805,7 +2782,7 @@
     </row>
     <row r="92" ht="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="97" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D97" s="10"/>
+      <c r="D97" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2820,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAFF2FEC-2B7E-4852-885C-A759096682C0}">
-  <dimension ref="A26:G55"/>
+  <dimension ref="A26:G52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2838,32 +2815,32 @@
   </cols>
   <sheetData>
     <row r="26" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="14">
         <v>0</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="15" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -2896,7 +2873,7 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="A31" s="14">
         <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2908,7 +2885,7 @@
       <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="A32" s="14">
         <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2919,100 +2896,110 @@
       </c>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:7" ht="33" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>7</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
-        <v>6</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>7</v>
-      </c>
-      <c r="B35" s="3" t="s">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
-        <v>8</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="4" t="s">
+      <c r="D39" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="C40" s="3" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>4</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -3020,13 +3007,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>113</v>
@@ -3037,16 +3024,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>114</v>
+        <v>31</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
@@ -3054,16 +3041,16 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>111</v>
+        <v>32</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>108</v>
+        <v>33</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>115</v>
+        <v>34</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
@@ -3071,16 +3058,16 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
@@ -3088,16 +3075,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -3105,16 +3092,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -3122,16 +3109,16 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -3139,16 +3126,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -3156,10 +3143,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>33</v>
@@ -3173,16 +3160,16 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -3190,76 +3177,25 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>13</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
-        <v>14</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
-        <v>15</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3270,7 +3206,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AB9B7F-5532-466A-8C88-B1D000186150}">
   <dimension ref="A31:G105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
@@ -3289,13 +3225,13 @@
   </cols>
   <sheetData>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -3385,19 +3321,19 @@
         <v>58</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -3586,19 +3522,19 @@
         <v>33</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="28" t="s">
+      <c r="A87" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B87" s="28"/>
-      <c r="C87" s="28"/>
-      <c r="D87" s="28"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
@@ -3667,7 +3603,7 @@
         <v>4</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>12</v>
@@ -3679,23 +3615,23 @@
         <v>5</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D94" s="3"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="28" t="s">
+      <c r="A96" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
+      <c r="G96" s="27"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
@@ -3833,7 +3769,7 @@
         <v>33</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
@@ -3844,13 +3780,13 @@
         <v>8</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
@@ -3890,30 +3826,30 @@
   </cols>
   <sheetData>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="17" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
-        <v>127</v>
+      <c r="A24" s="18" t="s">
+        <v>125</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>81</v>
@@ -3921,11 +3857,11 @@
       <c r="C24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="18"/>
+      <c r="D24" s="17"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>128</v>
+      <c r="A25" s="18" t="s">
+        <v>126</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>81</v>
@@ -3933,66 +3869,66 @@
       <c r="C25" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D25" s="18"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="18" t="s">
+      <c r="B27" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="18"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="19" t="s">
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="18"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="18"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="36"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E32" s="3" t="s">
@@ -4006,75 +3942,75 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+      <c r="A33" s="16">
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+      <c r="A34" s="16">
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
+        <v>3</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
+        <v>4</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D34" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
-        <v>3</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <v>4</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+      <c r="A37" s="16">
         <v>5</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -4086,21 +4022,21 @@
       <c r="D37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C38" s="18" t="s">
+      <c r="A38" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E38" s="3"/>
@@ -4108,8 +4044,8 @@
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>136</v>
+      <c r="A39" s="16" t="s">
+        <v>134</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>32</v>
@@ -4125,119 +4061,119 @@
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>137</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>139</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="D41" s="18" t="s">
-        <v>141</v>
+      <c r="A41" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>139</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="C42" s="18" t="s">
+      <c r="A42" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="18" t="s">
-        <v>147</v>
+      <c r="D42" s="17" t="s">
+        <v>145</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>142</v>
+      <c r="A43" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="C43" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="C44" s="18" t="s">
+      <c r="A44" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C44" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C45" s="18" t="s">
+      <c r="A45" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="17" t="s">
         <v>36</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B46" s="18" t="s">
+      <c r="A46" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -4275,12 +4211,12 @@
   </cols>
   <sheetData>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
@@ -4301,10 +4237,10 @@
         <v>0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>158</v>
+        <v>155</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>156</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -4313,10 +4249,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>171</v>
+        <v>157</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -4325,10 +4261,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>172</v>
+        <v>161</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>170</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -4337,10 +4273,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -4349,10 +4285,10 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D38" s="3"/>
     </row>
@@ -4361,10 +4297,10 @@
         <v>5</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -4373,10 +4309,10 @@
         <v>6</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>173</v>
+        <v>162</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -4385,10 +4321,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>174</v>
+        <v>163</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -4397,10 +4333,10 @@
         <v>8</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>175</v>
+        <v>164</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>173</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -4409,10 +4345,10 @@
         <v>9</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>176</v>
+        <v>165</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>174</v>
       </c>
       <c r="D43" s="3"/>
     </row>
@@ -4421,10 +4357,10 @@
         <v>10</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>177</v>
+        <v>166</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>175</v>
       </c>
       <c r="D44" s="3"/>
     </row>
@@ -4445,10 +4381,10 @@
         <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>181</v>
+        <v>158</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="D46" s="3"/>
     </row>
@@ -4457,35 +4393,35 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>182</v>
+        <v>159</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="37"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B50" s="18" t="s">
+      <c r="B50" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="18" t="s">
+      <c r="D50" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E50" s="3" t="s">
@@ -4502,13 +4438,13 @@
       <c r="A51" s="3">
         <v>1</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="C51" s="18" t="s">
+      <c r="B51" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C51" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="D51" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E51" s="3"/>
@@ -4519,33 +4455,33 @@
       <c r="A52" s="3">
         <v>2</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C52" s="18" t="s">
+      <c r="B52" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="18" t="s">
-        <v>193</v>
+      <c r="D52" s="17" t="s">
+        <v>191</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
-      <c r="G52" s="20" t="s">
-        <v>277</v>
+      <c r="G52" s="19" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>3</v>
       </c>
-      <c r="B53" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C53" s="18" t="s">
+      <c r="B53" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="18" t="s">
-        <v>194</v>
+      <c r="D53" s="17" t="s">
+        <v>192</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -4555,14 +4491,14 @@
       <c r="A54" s="3">
         <v>4</v>
       </c>
-      <c r="B54" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" s="18" t="s">
+      <c r="B54" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="18" t="s">
-        <v>195</v>
+      <c r="D54" s="17" t="s">
+        <v>193</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -4572,14 +4508,14 @@
       <c r="A55" s="3">
         <v>5</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" s="18" t="s">
+      <c r="B55" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="18" t="s">
-        <v>196</v>
+      <c r="D55" s="17" t="s">
+        <v>194</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -4589,14 +4525,14 @@
       <c r="A56" s="3">
         <v>6</v>
       </c>
-      <c r="B56" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C56" s="18" t="s">
+      <c r="B56" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D56" s="18" t="s">
-        <v>197</v>
+      <c r="D56" s="17" t="s">
+        <v>195</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -4606,14 +4542,14 @@
       <c r="A57" s="3">
         <v>7</v>
       </c>
-      <c r="B57" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="C57" s="18" t="s">
+      <c r="B57" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C57" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D57" s="18" t="s">
-        <v>198</v>
+      <c r="D57" s="17" t="s">
+        <v>196</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -4623,14 +4559,14 @@
       <c r="A58" s="3">
         <v>8</v>
       </c>
-      <c r="B58" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="C58" s="18" t="s">
+      <c r="B58" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C58" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D58" s="18" t="s">
-        <v>199</v>
+      <c r="D58" s="17" t="s">
+        <v>197</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -4640,14 +4576,14 @@
       <c r="A59" s="3">
         <v>9</v>
       </c>
-      <c r="B59" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="C59" s="18" t="s">
+      <c r="B59" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C59" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D59" s="18" t="s">
-        <v>200</v>
+      <c r="D59" s="17" t="s">
+        <v>198</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -4657,14 +4593,14 @@
       <c r="A60" s="3">
         <v>10</v>
       </c>
-      <c r="B60" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="C60" s="18" t="s">
+      <c r="B60" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D60" s="18" t="s">
-        <v>201</v>
+      <c r="D60" s="17" t="s">
+        <v>199</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -4674,14 +4610,14 @@
       <c r="A61" s="3">
         <v>11</v>
       </c>
-      <c r="B61" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C61" s="18" t="s">
+      <c r="B61" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C61" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D61" s="18" t="s">
-        <v>202</v>
+      <c r="D61" s="17" t="s">
+        <v>200</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -4692,13 +4628,13 @@
         <v>12</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -4709,13 +4645,13 @@
         <v>13</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -4726,13 +4662,13 @@
         <v>14</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -4743,13 +4679,13 @@
         <v>15</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -4760,13 +4696,13 @@
         <v>16</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -4777,13 +4713,13 @@
         <v>17</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -4793,14 +4729,14 @@
       <c r="A68" s="3">
         <v>18</v>
       </c>
-      <c r="B68" s="18" t="s">
-        <v>229</v>
+      <c r="B68" s="17" t="s">
+        <v>227</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>237</v>
+        <v>228</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>235</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -4810,14 +4746,14 @@
       <c r="A69" s="3">
         <v>19</v>
       </c>
-      <c r="B69" s="18" t="s">
-        <v>231</v>
+      <c r="B69" s="17" t="s">
+        <v>229</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>238</v>
+        <v>228</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>236</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -4827,14 +4763,14 @@
       <c r="A70" s="3">
         <v>20</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>232</v>
+      <c r="B70" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>239</v>
+        <v>228</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>237</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -4844,14 +4780,14 @@
       <c r="A71" s="3">
         <v>21</v>
       </c>
-      <c r="B71" s="18" t="s">
-        <v>233</v>
+      <c r="B71" s="17" t="s">
+        <v>231</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>240</v>
+        <v>228</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>238</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -4861,14 +4797,14 @@
       <c r="A72" s="3">
         <v>22</v>
       </c>
-      <c r="B72" s="18" t="s">
-        <v>234</v>
+      <c r="B72" s="17" t="s">
+        <v>232</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>241</v>
+        <v>228</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>239</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -4878,14 +4814,14 @@
       <c r="A73" s="3">
         <v>23</v>
       </c>
-      <c r="B73" s="18" t="s">
-        <v>235</v>
+      <c r="B73" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>240</v>
       </c>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -4895,14 +4831,14 @@
       <c r="A74" s="3">
         <v>24</v>
       </c>
-      <c r="B74" s="18" t="s">
-        <v>236</v>
+      <c r="B74" s="17" t="s">
+        <v>234</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>243</v>
+        <v>228</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>241</v>
       </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -4940,12 +4876,12 @@
   </cols>
   <sheetData>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -4966,10 +4902,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -4978,10 +4914,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -4990,10 +4926,10 @@
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D37" s="3"/>
     </row>
@@ -5002,10 +4938,10 @@
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D38" s="3"/>
     </row>
@@ -5014,10 +4950,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -5026,10 +4962,10 @@
         <v>5</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -5041,7 +4977,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -5050,10 +4986,10 @@
         <v>7</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -5062,35 +4998,35 @@
         <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>182</v>
+        <v>226</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -5107,13 +5043,13 @@
       <c r="A47" s="3">
         <v>1</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>135</v>
+      <c r="B47" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D47" s="18" t="s">
+      <c r="D47" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E47" s="3"/>
@@ -5124,33 +5060,33 @@
       <c r="A48" s="3">
         <v>2</v>
       </c>
-      <c r="B48" s="18" t="s">
-        <v>244</v>
+      <c r="B48" s="17" t="s">
+        <v>242</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>249</v>
+      <c r="D48" s="17" t="s">
+        <v>247</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
-      <c r="G48" s="21" t="s">
-        <v>278</v>
+      <c r="G48" s="20" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>3</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>245</v>
+      <c r="B49" s="17" t="s">
+        <v>243</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="18" t="s">
-        <v>250</v>
+      <c r="D49" s="17" t="s">
+        <v>248</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -5160,14 +5096,14 @@
       <c r="A50" s="3">
         <v>4</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>246</v>
+      <c r="B50" s="17" t="s">
+        <v>244</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>297</v>
+      <c r="D50" s="17" t="s">
+        <v>295</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -5177,33 +5113,33 @@
       <c r="A51" s="3">
         <v>5</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>247</v>
+      <c r="B51" s="17" t="s">
+        <v>245</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>251</v>
+      <c r="D51" s="17" t="s">
+        <v>249</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>6</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>248</v>
+      <c r="B52" s="17" t="s">
+        <v>246</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="18" t="s">
-        <v>252</v>
+      <c r="D52" s="17" t="s">
+        <v>250</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -5213,14 +5149,14 @@
       <c r="A53" s="3">
         <v>7</v>
       </c>
-      <c r="B53" s="18" t="s">
-        <v>256</v>
+      <c r="B53" s="17" t="s">
+        <v>254</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="18" t="s">
-        <v>255</v>
+      <c r="D53" s="17" t="s">
+        <v>253</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
@@ -5231,13 +5167,13 @@
         <v>8</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -5247,14 +5183,14 @@
       <c r="A55" s="3">
         <v>9</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>257</v>
+      <c r="B55" s="17" t="s">
+        <v>255</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D55" s="18" t="s">
-        <v>238</v>
+        <v>228</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>236</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -5264,14 +5200,14 @@
       <c r="A56" s="3">
         <v>10</v>
       </c>
-      <c r="B56" s="18" t="s">
-        <v>258</v>
+      <c r="B56" s="17" t="s">
+        <v>256</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D56" s="18" t="s">
-        <v>239</v>
+        <v>228</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>237</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -5281,14 +5217,14 @@
       <c r="A57" s="3">
         <v>11</v>
       </c>
-      <c r="B57" s="18" t="s">
-        <v>259</v>
+      <c r="B57" s="17" t="s">
+        <v>257</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>240</v>
+        <v>228</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>238</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -5298,14 +5234,14 @@
       <c r="A58" s="3">
         <v>12</v>
       </c>
-      <c r="B58" s="18" t="s">
-        <v>260</v>
+      <c r="B58" s="17" t="s">
+        <v>258</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>240</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -5316,13 +5252,13 @@
         <v>13</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>143</v>
+        <v>259</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -5333,13 +5269,13 @@
         <v>14</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -5350,7 +5286,7 @@
         <v>15</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>33</v>
@@ -5367,13 +5303,13 @@
         <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -5384,13 +5320,13 @@
         <v>17</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
@@ -5401,13 +5337,13 @@
         <v>18</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -5418,13 +5354,13 @@
         <v>19</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -5435,13 +5371,13 @@
         <v>20</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -5452,13 +5388,13 @@
         <v>21</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -5493,12 +5429,12 @@
   </cols>
   <sheetData>
     <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
     </row>
     <row r="34" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -5519,10 +5455,10 @@
         <v>0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D35" s="3"/>
     </row>
@@ -5531,10 +5467,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D36" s="3"/>
     </row>
@@ -5543,22 +5479,22 @@
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
+      <c r="A38" s="21">
         <v>3</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
@@ -5566,10 +5502,10 @@
         <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D39" s="3"/>
     </row>
@@ -5578,10 +5514,10 @@
         <v>5</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -5593,7 +5529,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D41" s="3"/>
     </row>
@@ -5605,7 +5541,7 @@
         <v>15</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D42" s="3"/>
     </row>
@@ -5614,10 +5550,10 @@
         <v>8</v>
       </c>
       <c r="B43" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C43" s="4" t="s">
         <v>288</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>290</v>
       </c>
       <c r="D43" s="3"/>
     </row>
@@ -5626,35 +5562,35 @@
         <v>9</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>182</v>
+        <v>226</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>180</v>
       </c>
       <c r="D44" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="37" t="s">
+      <c r="A47" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D48" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -5671,13 +5607,13 @@
       <c r="A49" s="3">
         <v>1</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>135</v>
+      <c r="B49" s="17" t="s">
+        <v>133</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="17" t="s">
         <v>37</v>
       </c>
       <c r="E49" s="3"/>
@@ -5688,33 +5624,33 @@
       <c r="A50" s="3">
         <v>2</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>291</v>
+      <c r="B50" s="17" t="s">
+        <v>289</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D50" s="18" t="s">
-        <v>292</v>
+      <c r="D50" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="21" t="s">
-        <v>293</v>
+      <c r="G50" s="20" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>3</v>
       </c>
-      <c r="B51" s="18" t="s">
-        <v>294</v>
+      <c r="B51" s="17" t="s">
+        <v>292</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="18" t="s">
-        <v>295</v>
+      <c r="D51" s="17" t="s">
+        <v>293</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
@@ -5724,14 +5660,14 @@
       <c r="A52" s="3">
         <v>4</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>190</v>
+      <c r="B52" s="17" t="s">
+        <v>188</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="18" t="s">
-        <v>296</v>
+      <c r="D52" s="17" t="s">
+        <v>294</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -5741,33 +5677,33 @@
       <c r="A53" s="3">
         <v>5</v>
       </c>
-      <c r="B53" s="18" t="s">
-        <v>247</v>
+      <c r="B53" s="17" t="s">
+        <v>245</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D53" s="18" t="s">
-        <v>251</v>
+      <c r="D53" s="17" t="s">
+        <v>249</v>
       </c>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>6</v>
       </c>
-      <c r="B54" s="18" t="s">
-        <v>191</v>
+      <c r="B54" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D54" s="18" t="s">
-        <v>201</v>
+      <c r="D54" s="17" t="s">
+        <v>199</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
@@ -5777,14 +5713,14 @@
       <c r="A55" s="3">
         <v>7</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>256</v>
+      <c r="B55" s="17" t="s">
+        <v>254</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D55" s="18" t="s">
-        <v>255</v>
+      <c r="D55" s="17" t="s">
+        <v>253</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -5795,13 +5731,13 @@
         <v>8</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>50</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -5811,14 +5747,14 @@
       <c r="A57" s="3">
         <v>9</v>
       </c>
-      <c r="B57" s="18" t="s">
-        <v>299</v>
+      <c r="B57" s="17" t="s">
+        <v>297</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D57" s="18" t="s">
-        <v>300</v>
+        <v>228</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>298</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
@@ -5828,14 +5764,14 @@
       <c r="A58" s="3">
         <v>10</v>
       </c>
-      <c r="B58" s="18" t="s">
-        <v>301</v>
+      <c r="B58" s="17" t="s">
+        <v>299</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D58" s="18" t="s">
-        <v>302</v>
+        <v>228</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>300</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
@@ -5845,14 +5781,14 @@
       <c r="A59" s="3">
         <v>11</v>
       </c>
-      <c r="B59" s="18" t="s">
-        <v>234</v>
+      <c r="B59" s="17" t="s">
+        <v>232</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>303</v>
+        <v>228</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>301</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -5862,14 +5798,14 @@
       <c r="A60" s="3">
         <v>12</v>
       </c>
-      <c r="B60" s="18" t="s">
-        <v>235</v>
+      <c r="B60" s="17" t="s">
+        <v>233</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="D60" s="18" t="s">
-        <v>242</v>
+        <v>228</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>240</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
@@ -5880,13 +5816,13 @@
         <v>13</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>143</v>
+        <v>259</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>141</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
@@ -5897,13 +5833,13 @@
         <v>14</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
@@ -5914,7 +5850,7 @@
         <v>15</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>33</v>
@@ -5931,13 +5867,13 @@
         <v>16</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
@@ -5948,13 +5884,13 @@
         <v>17</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
@@ -5965,13 +5901,13 @@
         <v>18</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -5982,81 +5918,81 @@
         <v>19</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="23">
+      <c r="A68" s="22">
         <v>20</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
     <row r="69" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A69" s="23">
+      <c r="A69" s="22">
         <v>21</v>
       </c>
-      <c r="B69" s="23" t="s">
-        <v>315</v>
-      </c>
-      <c r="C69" s="23" t="s">
+      <c r="B69" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C69" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
     <row r="70" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A70" s="23">
+      <c r="A70" s="22">
         <v>22</v>
       </c>
-      <c r="B70" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="C70" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="D70" s="23" t="s">
-        <v>318</v>
+      <c r="B70" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="C70" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="D70" s="22" t="s">
+        <v>316</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
     <row r="71" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="23">
+      <c r="A71" s="22">
         <v>23</v>
       </c>
-      <c r="B71" s="23" t="s">
-        <v>319</v>
-      </c>
-      <c r="C71" s="23" t="s">
+      <c r="B71" s="22" t="s">
+        <v>317</v>
+      </c>
+      <c r="C71" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>

</xml_diff>